<commit_message>
Change wiclient and wheel diameter settings
Add check for wheel diameter to workflow.
Layout runs for engine 213.
</commit_message>
<xml_diff>
--- a/measurements/Roster/TestTemplate.xlsx
+++ b/measurements/Roster/TestTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\PurpleHatModule\measurements\Roster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6453AD-4A6F-4EE3-B0B2-73F4B30C7D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822E3307-03FF-4667-BD28-DC0B2816E16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="645" windowWidth="27330" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="1650" windowWidth="27330" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>x</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Check (CV9 ) Motor control frequency and EMF sampling rate (default 0)</t>
+  </si>
+  <si>
+    <t>Check the wheel diameter:  30.69 mm</t>
   </si>
 </sst>
 </file>
@@ -26053,79 +26056,83 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26216,7 +26223,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>142873</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -26254,7 +26261,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -26824,13 +26831,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>16</xdr:row>
+          <xdr:row>17</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>16</xdr:row>
+          <xdr:row>17</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -26891,13 +26898,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>19</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>19</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -26958,13 +26965,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27025,13 +27032,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27092,13 +27099,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>24</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>24</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27293,13 +27300,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27360,13 +27367,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>22</xdr:row>
+          <xdr:row>23</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>22</xdr:row>
+          <xdr:row>23</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27427,13 +27434,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>23</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>23</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27490,14 +27497,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="200025" cy="161925"/>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>381000</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3093" name="Check Box 21" hidden="1">
@@ -27506,7 +27518,7 @@
                   <a14:compatExt spid="_x0000_s3093"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B07554F4-DFBF-4E21-B628-C09A604A4F00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000150C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -27546,7 +27558,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -27560,7 +27572,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -27568,7 +27580,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2E67985-C221-8ECD-4D27-18D72088835A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27586,6 +27598,73 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>180975</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>381000</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3094" name="Check Box 22" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3094"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{257DD1BC-AC53-4758-A0D6-61C1494B590C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -28044,10 +28123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28133,41 +28212,46 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>26</v>
       </c>
     </row>
@@ -28362,13 +28446,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>180975</xdr:colOff>
-                    <xdr:row>16</xdr:row>
+                    <xdr:row>17</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>381000</xdr:colOff>
-                    <xdr:row>16</xdr:row>
+                    <xdr:row>17</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28379,28 +28463,6 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="3084" r:id="rId12" name="Check Box 12">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>180975</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>381000</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="3085" r:id="rId13" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -28422,19 +28484,41 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
+            <control shapeId="3085" r:id="rId13" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>381000</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
             <control shapeId="3086" r:id="rId14" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28450,13 +28534,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>180975</xdr:colOff>
-                    <xdr:row>24</xdr:row>
+                    <xdr:row>25</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>381000</xdr:colOff>
-                    <xdr:row>24</xdr:row>
+                    <xdr:row>25</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28516,13 +28600,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>180975</xdr:colOff>
-                    <xdr:row>17</xdr:row>
+                    <xdr:row>18</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>381000</xdr:colOff>
-                    <xdr:row>17</xdr:row>
+                    <xdr:row>18</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28538,13 +28622,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>22</xdr:row>
+                    <xdr:row>23</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>22</xdr:row>
+                    <xdr:row>23</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28560,13 +28644,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>23</xdr:row>
+                    <xdr:row>24</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>23</xdr:row>
+                    <xdr:row>24</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28596,6 +28680,28 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3094" r:id="rId22" name="Check Box 22">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>381000</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>

<commit_message>
Speed profiles for RhB 644 and RhB 649
</commit_message>
<xml_diff>
--- a/measurements/Roster/TestTemplate.xlsx
+++ b/measurements/Roster/TestTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\PurpleHatModule\measurements\Roster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F9CCB3-747F-4012-BDD3-0E4666D3CD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED45862-0337-4A1F-B155-DE64AD7DECE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9765" yWindow="780" windowWidth="27330" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="1290" windowWidth="27330" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>x</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Notes:</t>
+  </si>
+  <si>
+    <t>For Zimo check that CV135 Speed Regulation is set to 0 via On Main Programing.</t>
   </si>
 </sst>
 </file>
@@ -26110,6 +26113,10 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
@@ -26226,7 +26233,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>142873</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -26264,7 +26271,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -26834,13 +26841,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -26901,13 +26908,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -26968,13 +26975,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27035,13 +27042,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>21</xdr:row>
+          <xdr:row>22</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>21</xdr:row>
+          <xdr:row>22</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27102,13 +27109,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>25</xdr:row>
+          <xdr:row>26</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>25</xdr:row>
+          <xdr:row>26</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27303,13 +27310,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>19</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>19</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27370,13 +27377,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>23</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>23</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27437,13 +27444,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>24</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>24</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27575,7 +27582,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -27607,13 +27614,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>16</xdr:row>
+          <xdr:row>17</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>16</xdr:row>
+          <xdr:row>17</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27665,6 +27672,68 @@
         </xdr:sp>
         <xdr:clientData/>
       </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>180975</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="200025" cy="161925"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3095" name="Check Box 23" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3095"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF949A45-AD4F-400D-9713-E37C9CC291FB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -28126,10 +28195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28213,53 +28282,58 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>36</v>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>37</v>
       </c>
     </row>
@@ -28454,13 +28528,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>180975</xdr:colOff>
-                    <xdr:row>17</xdr:row>
+                    <xdr:row>18</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>381000</xdr:colOff>
-                    <xdr:row>17</xdr:row>
+                    <xdr:row>18</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28471,28 +28545,6 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="3084" r:id="rId12" name="Check Box 12">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>180975</xdr:colOff>
-                    <xdr:row>19</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>381000</xdr:colOff>
-                    <xdr:row>19</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="3085" r:id="rId13" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -28514,19 +28566,41 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
+            <control shapeId="3085" r:id="rId13" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>381000</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
             <control shapeId="3086" r:id="rId14" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>21</xdr:row>
+                    <xdr:row>22</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>21</xdr:row>
+                    <xdr:row>22</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28542,13 +28616,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>180975</xdr:colOff>
-                    <xdr:row>25</xdr:row>
+                    <xdr:row>26</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>381000</xdr:colOff>
-                    <xdr:row>25</xdr:row>
+                    <xdr:row>26</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28608,13 +28682,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>180975</xdr:colOff>
-                    <xdr:row>18</xdr:row>
+                    <xdr:row>19</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>381000</xdr:colOff>
-                    <xdr:row>18</xdr:row>
+                    <xdr:row>19</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28630,13 +28704,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>23</xdr:row>
+                    <xdr:row>24</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>23</xdr:row>
+                    <xdr:row>24</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28652,13 +28726,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>24</xdr:row>
+                    <xdr:row>25</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>24</xdr:row>
+                    <xdr:row>25</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28696,13 +28770,35 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>180975</xdr:colOff>
-                    <xdr:row>16</xdr:row>
+                    <xdr:row>17</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>381000</xdr:colOff>
-                    <xdr:row>16</xdr:row>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3095" r:id="rId23" name="Check Box 23">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>381000</xdr:colOff>
+                    <xdr:row>15</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>

</xml_diff>

<commit_message>
Update template to include trims. Retake test for 616 to restore trims.
</commit_message>
<xml_diff>
--- a/measurements/Roster/TestTemplate.xlsx
+++ b/measurements/Roster/TestTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\PurpleHatModule\measurements\Roster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED45862-0337-4A1F-B155-DE64AD7DECE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43BAA5B-3FBD-46D3-8CFD-76001550ACB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="1290" windowWidth="27330" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10545" yWindow="405" windowWidth="27330" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>x</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>For Zimo check that CV135 Speed Regulation is set to 0 via On Main Programing.</t>
+  </si>
+  <si>
+    <t>Enter trims at the end of the speed table to save them…</t>
   </si>
 </sst>
 </file>
@@ -26117,6 +26120,10 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
@@ -26908,13 +26915,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -26975,13 +26982,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>21</xdr:row>
+          <xdr:row>22</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>21</xdr:row>
+          <xdr:row>22</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27042,13 +27049,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>22</xdr:row>
+          <xdr:row>23</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>22</xdr:row>
+          <xdr:row>23</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27109,13 +27116,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>26</xdr:row>
+          <xdr:row>27</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>26</xdr:row>
+          <xdr:row>27</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27377,13 +27384,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>24</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>24</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27444,13 +27451,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>25</xdr:row>
+          <xdr:row>26</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>25</xdr:row>
+          <xdr:row>26</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -27677,14 +27684,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>180975</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="200025" cy="161925"/>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>381000</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3095" name="Check Box 23" hidden="1">
@@ -27693,7 +27705,69 @@
                   <a14:compatExt spid="_x0000_s3095"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF949A45-AD4F-400D-9713-E37C9CC291FB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000170C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>180975</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="200025" cy="161925"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3096" name="Check Box 24" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3096"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FE09345-747C-4281-8A11-A15782289F00}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -28195,10 +28269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28304,36 +28378,41 @@
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>37</v>
       </c>
     </row>
@@ -28550,28 +28629,6 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>180975</xdr:colOff>
-                    <xdr:row>20</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>381000</xdr:colOff>
-                    <xdr:row>20</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="3085" r:id="rId13" name="Check Box 13">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>180975</xdr:colOff>
                     <xdr:row>21</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
@@ -28588,19 +28645,41 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
+            <control shapeId="3085" r:id="rId13" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>381000</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
             <control shapeId="3086" r:id="rId14" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>22</xdr:row>
+                    <xdr:row>23</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>22</xdr:row>
+                    <xdr:row>23</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28616,13 +28695,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>180975</xdr:colOff>
-                    <xdr:row>26</xdr:row>
+                    <xdr:row>27</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>381000</xdr:colOff>
-                    <xdr:row>26</xdr:row>
+                    <xdr:row>27</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28704,13 +28783,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>24</xdr:row>
+                    <xdr:row>25</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>24</xdr:row>
+                    <xdr:row>25</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28726,13 +28805,13 @@
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>25</xdr:row>
+                    <xdr:row>26</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>25</xdr:row>
+                    <xdr:row>26</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
@@ -28806,6 +28885,28 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3096" r:id="rId24" name="Check Box 24">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>381000</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>